<commit_message>
Made the groq usage for formatting
</commit_message>
<xml_diff>
--- a/umair_websites_to_scrap.xlsx
+++ b/umair_websites_to_scrap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="404">
   <si>
     <t>Category</t>
   </si>
@@ -1205,10 +1205,16 @@
     <t>WWW.YWINNIPEG.CA</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>Youth and Philanthropy Initiative Canada</t>
   </si>
   <si>
     <t>WWW.GOYPI.ORG</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Youth Science Canada</t>
@@ -1278,12 +1284,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1597,10 +1606,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3805,43 +3814,51 @@
       <c r="C184" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D184" s="2"/>
+      <c r="D184" s="2" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D185" s="2"/>
+        <v>398</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C186" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D186" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="D186" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D187" s="2"/>
+        <v>403</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>399</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
just corrected the funciton in main
</commit_message>
<xml_diff>
--- a/umair_websites_to_scrap.xlsx
+++ b/umair_websites_to_scrap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="408">
   <si>
     <t>Category</t>
   </si>
@@ -920,6 +920,9 @@
     <t>www.kwsphumane.ca</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>The Jane Goodall Institute of Canada</t>
   </si>
   <si>
@@ -944,6 +947,9 @@
     <t>WWW.PWRDF.ORG</t>
   </si>
   <si>
+    <t>No Events</t>
+  </si>
+  <si>
     <t>The Salvation Army in Canada</t>
   </si>
   <si>
@@ -989,6 +995,9 @@
     <t>www.vfwomenscentre.com</t>
   </si>
   <si>
+    <t>Pending</t>
+  </si>
+  <si>
     <t>The Vitanova Foundation</t>
   </si>
   <si>
@@ -1013,6 +1022,9 @@
     <t>WWW.THYROIDCANCERCANADA.ORG</t>
   </si>
   <si>
+    <t>Website Not Found</t>
+  </si>
+  <si>
     <t>Toronto Humane Society</t>
   </si>
   <si>
@@ -1151,18 +1163,12 @@
     <t>westparkfoundation.ca</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Whistler Community Services Society</t>
   </si>
   <si>
     <t>WWW.MYWCSS.ORG</t>
   </si>
   <si>
-    <t>No Events</t>
-  </si>
-  <si>
     <t>Women’s College Hospital Foundation</t>
   </si>
   <si>
@@ -1208,9 +1214,6 @@
     <t>YARMOUTHHOSPITALFOUNDATION.CA</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>YMCA - YWCA of Winnipeg</t>
   </si>
   <si>
@@ -1227,6 +1230,9 @@
   </si>
   <si>
     <t>WWW.YOUTHSCIENCE.CA</t>
+  </si>
+  <si>
+    <t>Large Site Scrapper needed</t>
   </si>
   <si>
     <t>Youth Without Shelter</t>
@@ -3253,464 +3259,540 @@
       <c r="C137" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D137" s="2"/>
+      <c r="D137" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D138" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D138" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D139" s="2"/>
+        <v>305</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D140" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D141" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C142" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D142" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D142" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D143" s="2"/>
+        <v>314</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D144" s="2"/>
+        <v>316</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D145" s="2"/>
+        <v>318</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D146" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D147" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D148" s="2"/>
+        <v>325</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D149" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D150" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D151" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D152" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D153" s="2"/>
+        <v>337</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D154" s="2"/>
+        <v>339</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D155" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D156" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D157" s="2"/>
+        <v>345</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D158" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="D159" s="2"/>
+        <v>349</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D160" s="2"/>
+        <v>351</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="D161" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="D162" s="2"/>
+        <v>355</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="D163" s="2"/>
+        <v>357</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D164" s="2"/>
+        <v>359</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D165" s="2"/>
+        <v>361</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D166" s="2"/>
+        <v>363</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D167" s="2"/>
+        <v>365</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D168" s="2"/>
+        <v>367</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="D169" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D170" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D171" s="2"/>
+        <v>373</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="D172" s="2"/>
+        <v>375</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D173" s="2"/>
+        <v>377</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="D174" s="2"/>
+        <v>379</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
@@ -3718,13 +3800,13 @@
         <v>23</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
@@ -3732,13 +3814,13 @@
         <v>163</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
@@ -3746,13 +3828,13 @@
         <v>163</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
@@ -3760,13 +3842,13 @@
         <v>92</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
@@ -3774,13 +3856,13 @@
         <v>32</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
@@ -3788,13 +3870,13 @@
         <v>92</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
@@ -3802,13 +3884,13 @@
         <v>63</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
@@ -3816,13 +3898,13 @@
         <v>163</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>397</v>
+        <v>326</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
@@ -3830,13 +3912,13 @@
         <v>23</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
@@ -3844,36 +3926,42 @@
         <v>26</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D185" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D186" s="2"/>
+        <v>404</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D187" s="2"/>
+        <v>407</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>301</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>